<commit_message>
control app, text with delect row
</commit_message>
<xml_diff>
--- a/external_info/data_orders.xlsx
+++ b/external_info/data_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,269 @@
           <t>id_scooter</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>id_scooter.1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>id_scooter.2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_scooter.3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>id_scooter.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>566-124</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>566-124</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>566-124</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>566-124</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>566-124</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>300-200</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>250-100</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>123-423</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>123-653</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>